<commit_message>
Update of Gantt chart
</commit_message>
<xml_diff>
--- a/ProjectManagement/Ganttchart.xlsx
+++ b/ProjectManagement/Ganttchart.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Selma\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Selma\Desktop\cpp_project\3D-ScannerProject\ProjectManagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,6 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -115,7 +114,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,6 +127,13 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -186,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -196,6 +202,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,8 +485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,8 +629,8 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="4"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
@@ -641,7 +648,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
+      <c r="I7" s="4"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
@@ -731,7 +738,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
-      <c r="I12" s="2"/>
+      <c r="I12" s="4"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>

</xml_diff>

<commit_message>
Week report + update Gantt chart
</commit_message>
<xml_diff>
--- a/ProjectManagement/Ganttchart.xlsx
+++ b/ProjectManagement/Ganttchart.xlsx
@@ -486,7 +486,7 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,9 +703,9 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
     </row>
@@ -741,7 +741,7 @@
       <c r="I12" s="4"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
+      <c r="L12" s="4"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
     </row>

</xml_diff>